<commit_message>
Transfer zwischen Views, Excel, Datenbanken, Code insgesamt verbessert
</commit_message>
<xml_diff>
--- a/Files/Assetklassen.xlsx
+++ b/Files/Assetklassen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilsk\Desktop 3\eclipse\Repos\PortfolioBro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilsk\Desktop 3\eclipse\Repos\PortfolioBro\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AE7D58-FE8B-4A72-9334-384F3AEC24AA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EAB02C-9E41-4A4A-9ADE-1C4624180674}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="6936" activeTab="1" xr2:uid="{FEA06F17-6AF7-433B-B1B8-405D1725179F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Erw. Rendite</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>Immobilien</t>
-  </si>
-  <si>
-    <t>Liq2342332423uide Mittel</t>
   </si>
 </sst>
 </file>
@@ -515,7 +512,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>1E-4</v>

</xml_diff>